<commit_message>
MSWC_Top.SchDoc edited. New PINOUT.
</commit_message>
<xml_diff>
--- a/MSWC_AT90CAN_PINOUT.xlsx
+++ b/MSWC_AT90CAN_PINOUT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28095" windowHeight="18660"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-BS=BrakeStatus</t>
+WSBT=WeehlSpinBlockingTyres</t>
         </r>
       </text>
     </comment>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
   <si>
     <t>AT90CAN-PIN</t>
   </si>
@@ -229,51 +229,6 @@
     <t>PF7</t>
   </si>
   <si>
-    <t>RGBLED_1.R</t>
-  </si>
-  <si>
-    <t>RGBLED_1.G</t>
-  </si>
-  <si>
-    <t>RGBLED_1.B</t>
-  </si>
-  <si>
-    <t>RGBLED_2.R</t>
-  </si>
-  <si>
-    <t>RGBLED_2.G</t>
-  </si>
-  <si>
-    <t>RGBLED_2.B</t>
-  </si>
-  <si>
-    <t>RGBLED_3.R</t>
-  </si>
-  <si>
-    <t>RGBLED_3.G</t>
-  </si>
-  <si>
-    <t>RGBLED_3.B</t>
-  </si>
-  <si>
-    <t>RGBLED_4.R</t>
-  </si>
-  <si>
-    <t>RGBLED_4.G</t>
-  </si>
-  <si>
-    <t>RGBLED_4.B</t>
-  </si>
-  <si>
-    <t>RGBLED_5.R</t>
-  </si>
-  <si>
-    <t>RGBLED_5.G</t>
-  </si>
-  <si>
-    <t>RGBLED_5.B</t>
-  </si>
-  <si>
     <t>Button_1</t>
   </si>
   <si>
@@ -316,79 +271,109 @@
     <t>Shifter_4</t>
   </si>
   <si>
+    <t>Foult</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>TX_CAN</t>
+  </si>
+  <si>
+    <t>RX_CAN</t>
+  </si>
+  <si>
+    <t>JTAG_TCK</t>
+  </si>
+  <si>
+    <t>JTAG_TMS</t>
+  </si>
+  <si>
+    <t>JTAG_TDO</t>
+  </si>
+  <si>
+    <t>JTAG_TDI</t>
+  </si>
+  <si>
+    <t>PG3</t>
+  </si>
+  <si>
+    <t>PG4</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>XTAL2</t>
+  </si>
+  <si>
+    <t>XTAL1</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>AVCC</t>
+  </si>
+  <si>
+    <t>AREF</t>
+  </si>
+  <si>
+    <t>PG2</t>
+  </si>
+  <si>
+    <t>PG1</t>
+  </si>
+  <si>
+    <t>PG0</t>
+  </si>
+  <si>
+    <t>LED1_WSBT</t>
+  </si>
+  <si>
+    <t>LED2_WSBT</t>
+  </si>
+  <si>
+    <t>RGLED_1.R</t>
+  </si>
+  <si>
+    <t>RGLED_1.G</t>
+  </si>
+  <si>
+    <t>RGLED_2.R</t>
+  </si>
+  <si>
+    <t>RGLED_2.G</t>
+  </si>
+  <si>
+    <t>RGLED_3.R</t>
+  </si>
+  <si>
+    <t>RGLED_3.G</t>
+  </si>
+  <si>
+    <t>RGLED_4.R</t>
+  </si>
+  <si>
+    <t>RGLED_4.G</t>
+  </si>
+  <si>
+    <t>RGLED_5.R</t>
+  </si>
+  <si>
+    <t>RGLED_5.G</t>
+  </si>
+  <si>
     <t>LED_Button_1</t>
   </si>
   <si>
     <t>LED_Button_2</t>
-  </si>
-  <si>
-    <t>LED_WSBT</t>
-  </si>
-  <si>
-    <t>Foult</t>
-  </si>
-  <si>
-    <t>Heart</t>
-  </si>
-  <si>
-    <t>TX_CAN</t>
-  </si>
-  <si>
-    <t>RX_CAN</t>
-  </si>
-  <si>
-    <t>JTAG_TCK</t>
-  </si>
-  <si>
-    <t>JTAG_TMS</t>
-  </si>
-  <si>
-    <t>JTAG_TDO</t>
-  </si>
-  <si>
-    <t>JTAG_TDI</t>
-  </si>
-  <si>
-    <t>LED_BS</t>
-  </si>
-  <si>
-    <t>PG3</t>
-  </si>
-  <si>
-    <t>PG4</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>VCC</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>XTAL2</t>
-  </si>
-  <si>
-    <t>XTAL1</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>AVCC</t>
-  </si>
-  <si>
-    <t>AREF</t>
-  </si>
-  <si>
-    <t>PG2</t>
-  </si>
-  <si>
-    <t>PG1</t>
-  </si>
-  <si>
-    <t>PG0</t>
   </si>
 </sst>
 </file>
@@ -785,7 +770,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="35.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,12 +801,12 @@
     </row>
     <row r="2" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="4"/>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="F2" s="4"/>
     </row>
@@ -828,11 +815,11 @@
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -841,11 +828,11 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -854,14 +841,14 @@
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -870,14 +857,14 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -886,14 +873,14 @@
         <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -902,14 +889,14 @@
         <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F8" s="4"/>
     </row>
@@ -918,14 +905,14 @@
         <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="F9" s="4"/>
     </row>
@@ -934,14 +921,14 @@
         <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -950,14 +937,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4"/>
     </row>
@@ -965,12 +952,15 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -980,7 +970,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -989,11 +979,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -1002,14 +992,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -1018,14 +1008,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -1034,7 +1024,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
@@ -1058,96 +1048,78 @@
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F26" s="4"/>
     </row>
@@ -1156,14 +1128,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F27" s="4"/>
     </row>
@@ -1172,14 +1144,14 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F28" s="4"/>
     </row>
@@ -1188,14 +1160,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F29" s="4"/>
     </row>
@@ -1204,14 +1176,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F30" s="4"/>
     </row>
@@ -1230,14 +1202,14 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F32" s="4"/>
     </row>
@@ -1246,11 +1218,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F33" s="4"/>
     </row>
@@ -1260,7 +1232,7 @@
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="2" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="F34" s="4"/>
     </row>

</xml_diff>